<commit_message>
New features are added
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -473,7 +473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1d84bec9-8fdb-49dc-8ed7-8e2fd5038f1d}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5c924da8-4d4c-4749-bb5c-5bdc0972d1e5}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42dd6e1c-067b-476c-9e67-ffac601af4c8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0704df28-e06c-467b-9c9e-b63cd31debb9}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>

</xml_diff>

<commit_message>
Data fetching for json and xml is done
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -473,7 +473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5c924da8-4d4c-4749-bb5c-5bdc0972d1e5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e2ea3465-ee0e-4311-a858-a26378f95de8}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0704df28-e06c-467b-9c9e-b63cd31debb9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ef8e0ab0-ae39-40e2-a6c6-69de43e28aa2}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>

</xml_diff>